<commit_message>
Updating form to test data type checks
</commit_message>
<xml_diff>
--- a/test/sample_forms/Form-1DI.xlsx
+++ b/test/sample_forms/Form-1DI.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\dev\git\BitBucket workspaces\IOTC-ws\R libs\base\forms\base-form-management\test\test_forms\samples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\dev\git\BitBucket workspaces\IOTC-ws\R libs\base\forms\base-form-management\test\sample_forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE4C1B80-EEBA-4BD8-A62E-D40F16F7ADCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D695AF28-D355-4C43-8AA5-DC8170563E9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Z3raniWjLRXszYCbzXa/TU1R8wd1kHrHNccmNn7mHkAZRDJmvrP7BMraCIbrDBSr6tBMzuhQ6TxYUg6cyC/1Bg==" workbookSaltValue="C01nC0I7gdRYfsDcA3RybQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="1140" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="90">
   <si>
     <t>Focal point</t>
   </si>
@@ -326,6 +326,12 @@
   </si>
   <si>
     <t>HL-AF[IN]TR</t>
+  </si>
+  <si>
+    <t>UN</t>
+  </si>
+  <si>
+    <t>PA</t>
   </si>
 </sst>
 </file>
@@ -1964,7 +1970,7 @@
       <pane xSplit="11" ySplit="7" topLeftCell="L8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomRight" activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3920,7 +3926,7 @@
         <v>80</v>
       </c>
       <c r="F11" s="32" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="G11" s="33" t="s">
         <v>75</v>
@@ -4094,7 +4100,7 @@
       <c r="D13" s="33"/>
       <c r="E13" s="50"/>
       <c r="F13" s="32" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G13" s="33" t="s">
         <v>75</v>
@@ -4628,7 +4634,7 @@
         <v>80</v>
       </c>
       <c r="F19" s="32" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G19" s="33" t="s">
         <v>75</v>
@@ -4717,7 +4723,7 @@
         <v>78</v>
       </c>
       <c r="F20" s="32" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G20" s="33" t="s">
         <v>75</v>
@@ -5260,7 +5266,7 @@
         <v>78</v>
       </c>
       <c r="F27" s="32" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="G27" s="33" t="s">
         <v>83</v>

</xml_diff>